<commit_message>
actualizacion de archivos camiones y asociados, e inclusion de algoritmo de optimizacion
actualizacion de archivos camiones y asociados, e inclusion de algoritmo
de optimizacion
</commit_message>
<xml_diff>
--- a/Archivos_Excel_Matrices/Matriz de camiones.xlsx
+++ b/Archivos_Excel_Matrices/Matriz de camiones.xlsx
@@ -15,7 +15,7 @@
     <sheet name="Info camiones" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'Info camiones'!$B$3:$I$22</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'Info camiones'!$B$3:$H$21</definedName>
   </definedNames>
   <calcPr calcId="152511"/>
 </workbook>
@@ -56,14 +56,11 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="16">
   <si>
     <t>Placa</t>
   </si>
   <si>
-    <t>Campos</t>
-  </si>
-  <si>
     <t>Osvaldo</t>
   </si>
   <si>
@@ -85,34 +82,28 @@
     <t>Cap por campo (q)</t>
   </si>
   <si>
-    <t>Cap por campo (kg)</t>
-  </si>
-  <si>
     <t>Proveedor</t>
   </si>
   <si>
     <t>Info camiones</t>
   </si>
   <si>
-    <t>?</t>
-  </si>
-  <si>
-    <t>#</t>
-  </si>
-  <si>
     <t>Utilización ideal</t>
   </si>
   <si>
     <t>Dos Pinos</t>
   </si>
   <si>
-    <t># entrega a la cual no puede ir</t>
-  </si>
-  <si>
-    <t xml:space="preserve"># </t>
-  </si>
-  <si>
-    <t>Capacidad</t>
+    <t>Cantidad de compartimientos por camión</t>
+  </si>
+  <si>
+    <t>Capacidad por compartimiento (kg)</t>
+  </si>
+  <si>
+    <t>Capacidad total del camión</t>
+  </si>
+  <si>
+    <t>Cantidad de camiones</t>
   </si>
 </sst>
 </file>
@@ -161,18 +152,12 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="2">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFF00"/>
-        <bgColor indexed="64"/>
-      </patternFill>
     </fill>
   </fills>
   <borders count="4">
@@ -230,21 +215,14 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="15">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="9" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -575,603 +553,516 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="B2:L22"/>
+  <dimension ref="B2:K21"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="G9" sqref="G9"/>
+      <selection activeCell="I1" sqref="I1:I1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="3.140625" style="1" customWidth="1"/>
-    <col min="2" max="2" width="4.140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="14.140625" style="1" customWidth="1"/>
     <col min="3" max="3" width="9.42578125" style="2" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="11.7109375" style="2" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="19.7109375" style="2" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="25.7109375" style="2" customWidth="1"/>
+    <col min="5" max="5" width="19.7109375" style="2" hidden="1" customWidth="1"/>
     <col min="6" max="6" width="20.42578125" style="2" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="13.28515625" style="2" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="15.5703125" style="2" customWidth="1"/>
     <col min="8" max="8" width="13.85546875" style="2" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="19.42578125" style="1" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="11.42578125" style="1"/>
-    <col min="11" max="11" width="14" style="1" bestFit="1" customWidth="1"/>
-    <col min="12" max="16384" width="11.42578125" style="1"/>
+    <col min="9" max="9" width="11.42578125" style="1"/>
+    <col min="10" max="10" width="14" style="1" bestFit="1" customWidth="1"/>
+    <col min="11" max="16384" width="11.42578125" style="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:12" x14ac:dyDescent="0.2">
-      <c r="B2" s="14" t="s">
-        <v>11</v>
-      </c>
-      <c r="C2" s="14"/>
-      <c r="D2" s="14"/>
-      <c r="E2" s="14"/>
-      <c r="F2" s="14"/>
-      <c r="G2" s="14"/>
-      <c r="H2" s="14"/>
-      <c r="I2" s="3"/>
-      <c r="K2" s="1" t="s">
+    <row r="2" spans="2:11" x14ac:dyDescent="0.2">
+      <c r="B2" s="11" t="s">
+        <v>9</v>
+      </c>
+      <c r="C2" s="11"/>
+      <c r="D2" s="11"/>
+      <c r="E2" s="11"/>
+      <c r="F2" s="11"/>
+      <c r="G2" s="11"/>
+      <c r="H2" s="11"/>
+      <c r="J2" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="K2" s="4">
+        <v>0.85</v>
+      </c>
+    </row>
+    <row r="3" spans="2:11" s="7" customFormat="1" ht="27.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B3" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="C3" s="5" t="s">
+        <v>0</v>
+      </c>
+      <c r="D3" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="E3" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="F3" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="G3" s="6" t="s">
         <v>14</v>
       </c>
-      <c r="L2" s="6">
-        <v>0.85</v>
-      </c>
-    </row>
-    <row r="3" spans="2:12" s="10" customFormat="1" ht="27.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B3" s="7" t="s">
-        <v>13</v>
-      </c>
-      <c r="C3" s="8" t="s">
-        <v>0</v>
-      </c>
-      <c r="D3" s="8" t="s">
-        <v>1</v>
-      </c>
-      <c r="E3" s="8" t="s">
+      <c r="H3" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="F3" s="8" t="s">
-        <v>9</v>
-      </c>
-      <c r="G3" s="8" t="s">
-        <v>18</v>
-      </c>
-      <c r="H3" s="8" t="s">
-        <v>10</v>
-      </c>
-      <c r="I3" s="9" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="4" spans="2:12" x14ac:dyDescent="0.2">
+    </row>
+    <row r="4" spans="2:11" x14ac:dyDescent="0.2">
       <c r="B4" s="3">
         <v>1</v>
       </c>
-      <c r="C4" s="11">
+      <c r="C4" s="8">
         <v>152388</v>
       </c>
-      <c r="D4" s="11">
-        <v>5</v>
-      </c>
-      <c r="E4" s="11">
-        <v>65</v>
-      </c>
-      <c r="F4" s="11">
+      <c r="D4" s="8">
+        <v>5</v>
+      </c>
+      <c r="E4" s="8">
+        <v>65</v>
+      </c>
+      <c r="F4" s="8">
         <f t="shared" ref="F4:F19" si="0">E4*46</f>
         <v>2990</v>
       </c>
-      <c r="G4" s="11">
+      <c r="G4" s="8">
         <f t="shared" ref="G4:G11" si="1">F4*D4</f>
         <v>14950</v>
       </c>
-      <c r="H4" s="11" t="s">
-        <v>15</v>
-      </c>
-      <c r="I4" s="11" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="5" spans="2:12" x14ac:dyDescent="0.2">
+      <c r="H4" s="8" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="5" spans="2:11" x14ac:dyDescent="0.2">
       <c r="B5" s="3">
         <v>2</v>
       </c>
-      <c r="C5" s="11">
+      <c r="C5" s="8">
         <v>152444</v>
       </c>
-      <c r="D5" s="11">
-        <v>5</v>
-      </c>
-      <c r="E5" s="11">
-        <v>65</v>
-      </c>
-      <c r="F5" s="11">
-        <f t="shared" si="0"/>
-        <v>2990</v>
-      </c>
-      <c r="G5" s="11">
+      <c r="D5" s="8">
+        <v>5</v>
+      </c>
+      <c r="E5" s="8">
+        <v>65</v>
+      </c>
+      <c r="F5" s="8">
+        <f t="shared" si="0"/>
+        <v>2990</v>
+      </c>
+      <c r="G5" s="8">
         <f t="shared" si="1"/>
         <v>14950</v>
       </c>
-      <c r="H5" s="11" t="s">
-        <v>15</v>
-      </c>
-      <c r="I5" s="11" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="6" spans="2:12" x14ac:dyDescent="0.2">
+      <c r="H5" s="8" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="6" spans="2:11" x14ac:dyDescent="0.2">
       <c r="B6" s="3">
         <v>3</v>
       </c>
-      <c r="C6" s="11">
+      <c r="C6" s="8">
         <v>152445</v>
       </c>
-      <c r="D6" s="11">
-        <v>5</v>
-      </c>
-      <c r="E6" s="11">
-        <v>65</v>
-      </c>
-      <c r="F6" s="11">
-        <f t="shared" si="0"/>
-        <v>2990</v>
-      </c>
-      <c r="G6" s="11">
+      <c r="D6" s="8">
+        <v>5</v>
+      </c>
+      <c r="E6" s="8">
+        <v>65</v>
+      </c>
+      <c r="F6" s="8">
+        <f t="shared" si="0"/>
+        <v>2990</v>
+      </c>
+      <c r="G6" s="8">
         <f t="shared" si="1"/>
         <v>14950</v>
       </c>
-      <c r="H6" s="11" t="s">
-        <v>15</v>
-      </c>
-      <c r="I6" s="11" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="7" spans="2:12" x14ac:dyDescent="0.2">
+      <c r="H6" s="8" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="7" spans="2:11" x14ac:dyDescent="0.2">
       <c r="B7" s="3">
         <v>4</v>
       </c>
-      <c r="C7" s="11">
+      <c r="C7" s="8">
         <v>156024</v>
       </c>
-      <c r="D7" s="11">
+      <c r="D7" s="8">
         <v>6</v>
       </c>
-      <c r="E7" s="11">
+      <c r="E7" s="8">
         <v>55</v>
       </c>
-      <c r="F7" s="11">
+      <c r="F7" s="8">
         <f t="shared" si="0"/>
         <v>2530</v>
       </c>
-      <c r="G7" s="11">
+      <c r="G7" s="8">
         <f t="shared" si="1"/>
         <v>15180</v>
       </c>
-      <c r="H7" s="11" t="s">
-        <v>15</v>
-      </c>
-      <c r="I7" s="11" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="8" spans="2:12" x14ac:dyDescent="0.2">
+      <c r="H7" s="8" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="8" spans="2:11" x14ac:dyDescent="0.2">
       <c r="B8" s="3">
         <v>5</v>
       </c>
-      <c r="C8" s="11">
+      <c r="C8" s="8">
         <v>158154</v>
       </c>
-      <c r="D8" s="11">
+      <c r="D8" s="8">
         <v>6</v>
       </c>
-      <c r="E8" s="11">
+      <c r="E8" s="8">
         <v>55</v>
       </c>
-      <c r="F8" s="11">
+      <c r="F8" s="8">
         <f t="shared" si="0"/>
         <v>2530</v>
       </c>
-      <c r="G8" s="11">
+      <c r="G8" s="8">
         <f t="shared" si="1"/>
         <v>15180</v>
       </c>
-      <c r="H8" s="11" t="s">
-        <v>15</v>
-      </c>
-      <c r="I8" s="11" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="9" spans="2:12" x14ac:dyDescent="0.2">
+      <c r="H8" s="8" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="9" spans="2:11" x14ac:dyDescent="0.2">
       <c r="B9" s="3">
         <v>6</v>
       </c>
-      <c r="C9" s="11">
+      <c r="C9" s="8">
         <v>158715</v>
       </c>
-      <c r="D9" s="11">
-        <v>5</v>
-      </c>
-      <c r="E9" s="11">
-        <v>65</v>
-      </c>
-      <c r="F9" s="11">
-        <f t="shared" si="0"/>
-        <v>2990</v>
-      </c>
-      <c r="G9" s="11">
+      <c r="D9" s="8">
+        <v>5</v>
+      </c>
+      <c r="E9" s="8">
+        <v>65</v>
+      </c>
+      <c r="F9" s="8">
+        <f t="shared" si="0"/>
+        <v>2990</v>
+      </c>
+      <c r="G9" s="8">
         <f t="shared" si="1"/>
         <v>14950</v>
       </c>
-      <c r="H9" s="11" t="s">
-        <v>15</v>
-      </c>
-      <c r="I9" s="11" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="10" spans="2:12" x14ac:dyDescent="0.2">
+      <c r="H9" s="8" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="10" spans="2:11" x14ac:dyDescent="0.2">
       <c r="B10" s="3">
         <v>7</v>
       </c>
-      <c r="C10" s="11">
+      <c r="C10" s="8">
         <v>159927</v>
       </c>
-      <c r="D10" s="11">
+      <c r="D10" s="8">
         <v>6</v>
       </c>
-      <c r="E10" s="11">
+      <c r="E10" s="8">
         <v>55</v>
       </c>
-      <c r="F10" s="11">
+      <c r="F10" s="8">
         <f t="shared" si="0"/>
         <v>2530</v>
       </c>
-      <c r="G10" s="11">
+      <c r="G10" s="8">
         <f t="shared" si="1"/>
         <v>15180</v>
       </c>
-      <c r="H10" s="11" t="s">
-        <v>15</v>
-      </c>
-      <c r="I10" s="11" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="11" spans="2:12" x14ac:dyDescent="0.2">
+      <c r="H10" s="8" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="11" spans="2:11" x14ac:dyDescent="0.2">
       <c r="B11" s="3">
         <v>8</v>
       </c>
-      <c r="C11" s="11">
+      <c r="C11" s="8">
         <v>159582</v>
       </c>
-      <c r="D11" s="11">
+      <c r="D11" s="8">
         <v>6</v>
       </c>
-      <c r="E11" s="11">
+      <c r="E11" s="8">
         <v>55</v>
       </c>
-      <c r="F11" s="11">
+      <c r="F11" s="8">
         <f t="shared" si="0"/>
         <v>2530</v>
       </c>
-      <c r="G11" s="11">
+      <c r="G11" s="8">
         <f t="shared" si="1"/>
         <v>15180</v>
       </c>
-      <c r="H11" s="11" t="s">
-        <v>15</v>
-      </c>
-      <c r="I11" s="11" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="12" spans="2:12" x14ac:dyDescent="0.2">
+      <c r="H11" s="8" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="12" spans="2:11" x14ac:dyDescent="0.2">
       <c r="B12" s="3">
         <v>9</v>
       </c>
-      <c r="C12" s="11">
+      <c r="C12" s="8">
         <v>134665</v>
       </c>
-      <c r="D12" s="11">
-        <v>5</v>
-      </c>
-      <c r="E12" s="11">
-        <v>65</v>
-      </c>
-      <c r="F12" s="11">
-        <f t="shared" si="0"/>
-        <v>2990</v>
-      </c>
-      <c r="G12" s="11">
+      <c r="D12" s="8">
+        <v>5</v>
+      </c>
+      <c r="E12" s="8">
+        <v>65</v>
+      </c>
+      <c r="F12" s="8">
+        <f t="shared" si="0"/>
+        <v>2990</v>
+      </c>
+      <c r="G12" s="8">
         <f t="shared" ref="G12:G19" si="2">E12*46*D12</f>
         <v>14950</v>
       </c>
-      <c r="H12" s="11" t="s">
-        <v>4</v>
-      </c>
-      <c r="I12" s="11" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="13" spans="2:12" x14ac:dyDescent="0.2">
+      <c r="H12" s="8" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="13" spans="2:11" x14ac:dyDescent="0.2">
       <c r="B13" s="3">
         <v>10</v>
       </c>
-      <c r="C13" s="11">
+      <c r="C13" s="8">
         <v>162343</v>
       </c>
-      <c r="D13" s="11">
-        <v>5</v>
-      </c>
-      <c r="E13" s="11">
-        <v>65</v>
-      </c>
-      <c r="F13" s="11">
-        <f t="shared" si="0"/>
-        <v>2990</v>
-      </c>
-      <c r="G13" s="11">
+      <c r="D13" s="8">
+        <v>5</v>
+      </c>
+      <c r="E13" s="8">
+        <v>65</v>
+      </c>
+      <c r="F13" s="8">
+        <f t="shared" si="0"/>
+        <v>2990</v>
+      </c>
+      <c r="G13" s="8">
         <f t="shared" si="2"/>
         <v>14950</v>
       </c>
-      <c r="H13" s="11" t="s">
-        <v>5</v>
-      </c>
-      <c r="I13" s="11" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="14" spans="2:12" x14ac:dyDescent="0.2">
+      <c r="H13" s="8" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="14" spans="2:11" x14ac:dyDescent="0.2">
       <c r="B14" s="3">
         <v>11</v>
       </c>
-      <c r="C14" s="11">
+      <c r="C14" s="8">
         <v>154914</v>
       </c>
-      <c r="D14" s="11">
+      <c r="D14" s="8">
         <v>6</v>
       </c>
-      <c r="E14" s="11">
-        <v>65</v>
-      </c>
-      <c r="F14" s="11">
-        <f t="shared" si="0"/>
-        <v>2990</v>
-      </c>
-      <c r="G14" s="11">
+      <c r="E14" s="8">
+        <v>65</v>
+      </c>
+      <c r="F14" s="8">
+        <f t="shared" si="0"/>
+        <v>2990</v>
+      </c>
+      <c r="G14" s="8">
         <f t="shared" si="2"/>
         <v>17940</v>
       </c>
-      <c r="H14" s="11" t="s">
-        <v>5</v>
-      </c>
-      <c r="I14" s="11" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="15" spans="2:12" x14ac:dyDescent="0.2">
+      <c r="H14" s="8" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="15" spans="2:11" x14ac:dyDescent="0.2">
       <c r="B15" s="3">
         <v>12</v>
       </c>
-      <c r="C15" s="11">
+      <c r="C15" s="8">
         <v>160522</v>
       </c>
-      <c r="D15" s="11">
-        <v>5</v>
-      </c>
-      <c r="E15" s="11">
-        <v>65</v>
-      </c>
-      <c r="F15" s="11">
-        <f t="shared" si="0"/>
-        <v>2990</v>
-      </c>
-      <c r="G15" s="11">
+      <c r="D15" s="8">
+        <v>5</v>
+      </c>
+      <c r="E15" s="8">
+        <v>65</v>
+      </c>
+      <c r="F15" s="8">
+        <f t="shared" si="0"/>
+        <v>2990</v>
+      </c>
+      <c r="G15" s="8">
         <f t="shared" si="2"/>
         <v>14950</v>
       </c>
-      <c r="H15" s="11" t="s">
-        <v>5</v>
-      </c>
-      <c r="I15" s="11" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="16" spans="2:12" x14ac:dyDescent="0.2">
+      <c r="H15" s="8" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="16" spans="2:11" x14ac:dyDescent="0.2">
       <c r="B16" s="3">
         <v>13</v>
       </c>
-      <c r="C16" s="11">
+      <c r="C16" s="8">
         <v>134388</v>
       </c>
-      <c r="D16" s="11">
+      <c r="D16" s="8">
         <v>6</v>
       </c>
-      <c r="E16" s="11">
-        <v>65</v>
-      </c>
-      <c r="F16" s="11">
-        <f t="shared" si="0"/>
-        <v>2990</v>
-      </c>
-      <c r="G16" s="11">
+      <c r="E16" s="8">
+        <v>65</v>
+      </c>
+      <c r="F16" s="8">
+        <f t="shared" si="0"/>
+        <v>2990</v>
+      </c>
+      <c r="G16" s="8">
         <f t="shared" si="2"/>
         <v>17940</v>
       </c>
-      <c r="H16" s="11" t="s">
-        <v>2</v>
-      </c>
-      <c r="I16" s="11" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="17" spans="2:9" x14ac:dyDescent="0.2">
+      <c r="H16" s="8" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="17" spans="2:8" x14ac:dyDescent="0.2">
       <c r="B17" s="3">
         <v>14</v>
       </c>
-      <c r="C17" s="11">
+      <c r="C17" s="8">
         <v>142746</v>
       </c>
-      <c r="D17" s="11">
-        <v>5</v>
-      </c>
-      <c r="E17" s="11">
-        <v>65</v>
-      </c>
-      <c r="F17" s="11">
-        <f t="shared" si="0"/>
-        <v>2990</v>
-      </c>
-      <c r="G17" s="11">
+      <c r="D17" s="8">
+        <v>5</v>
+      </c>
+      <c r="E17" s="8">
+        <v>65</v>
+      </c>
+      <c r="F17" s="8">
+        <f t="shared" si="0"/>
+        <v>2990</v>
+      </c>
+      <c r="G17" s="8">
         <f t="shared" si="2"/>
         <v>14950</v>
       </c>
-      <c r="H17" s="11" t="s">
-        <v>2</v>
-      </c>
-      <c r="I17" s="11" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="18" spans="2:9" x14ac:dyDescent="0.2">
+      <c r="H17" s="8" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="18" spans="2:8" x14ac:dyDescent="0.2">
       <c r="B18" s="3">
         <v>15</v>
       </c>
-      <c r="C18" s="11">
+      <c r="C18" s="8">
         <v>137418</v>
       </c>
-      <c r="D18" s="11">
+      <c r="D18" s="8">
         <v>6</v>
       </c>
-      <c r="E18" s="11">
-        <v>65</v>
-      </c>
-      <c r="F18" s="11">
-        <f t="shared" si="0"/>
-        <v>2990</v>
-      </c>
-      <c r="G18" s="11">
+      <c r="E18" s="8">
+        <v>65</v>
+      </c>
+      <c r="F18" s="8">
+        <f t="shared" si="0"/>
+        <v>2990</v>
+      </c>
+      <c r="G18" s="8">
         <f t="shared" si="2"/>
         <v>17940</v>
       </c>
-      <c r="H18" s="11" t="s">
-        <v>3</v>
-      </c>
-      <c r="I18" s="11" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="19" spans="2:9" x14ac:dyDescent="0.2">
+      <c r="H18" s="8" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="19" spans="2:8" x14ac:dyDescent="0.2">
       <c r="B19" s="3">
         <v>16</v>
       </c>
-      <c r="C19" s="11">
+      <c r="C19" s="8">
         <v>137443</v>
       </c>
-      <c r="D19" s="11">
+      <c r="D19" s="8">
         <v>6</v>
       </c>
-      <c r="E19" s="11">
-        <v>65</v>
-      </c>
-      <c r="F19" s="11">
-        <f t="shared" si="0"/>
-        <v>2990</v>
-      </c>
-      <c r="G19" s="11">
+      <c r="E19" s="8">
+        <v>65</v>
+      </c>
+      <c r="F19" s="8">
+        <f t="shared" si="0"/>
+        <v>2990</v>
+      </c>
+      <c r="G19" s="8">
         <f t="shared" si="2"/>
         <v>17940</v>
       </c>
-      <c r="H19" s="11" t="s">
-        <v>3</v>
-      </c>
-      <c r="I19" s="11" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="20" spans="2:9" x14ac:dyDescent="0.2">
+      <c r="H19" s="8" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="20" spans="2:8" x14ac:dyDescent="0.2">
       <c r="B20" s="3">
         <v>17</v>
       </c>
-      <c r="C20" s="11">
+      <c r="C20" s="8">
         <v>133391</v>
       </c>
-      <c r="D20" s="11">
-        <v>5</v>
-      </c>
-      <c r="E20" s="12" t="s">
-        <v>7</v>
-      </c>
-      <c r="F20" s="13"/>
-      <c r="G20" s="11">
+      <c r="D20" s="8">
+        <v>5</v>
+      </c>
+      <c r="E20" s="9" t="s">
+        <v>6</v>
+      </c>
+      <c r="F20" s="10"/>
+      <c r="G20" s="8">
         <f>(4*65*46)+(1*90*46)</f>
         <v>16100</v>
       </c>
-      <c r="H20" s="11" t="s">
-        <v>6</v>
-      </c>
-      <c r="I20" s="11" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="21" spans="2:9" x14ac:dyDescent="0.2">
+      <c r="H20" s="8" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="21" spans="2:8" x14ac:dyDescent="0.2">
       <c r="B21" s="3">
         <v>18</v>
       </c>
-      <c r="C21" s="11">
+      <c r="C21" s="8">
         <v>145985</v>
       </c>
-      <c r="D21" s="11">
-        <v>5</v>
-      </c>
-      <c r="E21" s="11">
-        <v>65</v>
-      </c>
-      <c r="F21" s="11">
+      <c r="D21" s="8">
+        <v>5</v>
+      </c>
+      <c r="E21" s="8">
+        <v>65</v>
+      </c>
+      <c r="F21" s="8">
         <f>E21*46</f>
         <v>2990</v>
       </c>
-      <c r="G21" s="11">
+      <c r="G21" s="8">
         <f>E21*46*D21</f>
         <v>14950</v>
       </c>
-      <c r="H21" s="11" t="s">
-        <v>6</v>
-      </c>
-      <c r="I21" s="11" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="22" spans="2:9" x14ac:dyDescent="0.2">
-      <c r="B22" s="4">
-        <v>19</v>
-      </c>
-      <c r="C22" s="5" t="s">
-        <v>12</v>
-      </c>
-      <c r="D22" s="5">
-        <v>5</v>
-      </c>
-      <c r="E22" s="5">
-        <v>65</v>
-      </c>
-      <c r="F22" s="5">
-        <f>E22*46</f>
-        <v>2990</v>
-      </c>
-      <c r="G22" s="5">
-        <f>E22*46*D22</f>
-        <v>14950</v>
-      </c>
-      <c r="H22" s="5" t="s">
-        <v>6</v>
-      </c>
-      <c r="I22" s="11" t="s">
-        <v>17</v>
+      <c r="H21" s="8" t="s">
+        <v>5</v>
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="B3:I22"/>
+  <autoFilter ref="B3:H21"/>
   <mergeCells count="2">
     <mergeCell ref="E20:F20"/>
     <mergeCell ref="B2:H2"/>

</xml_diff>

<commit_message>
Inicio de implementacion Segundo Algoritmo
- Se modifican los valores de precioFlete y montoFlete
- Se agrega la variable tiempo disponibilidad a los camiones
- Se crean las matrices de tiempos y distancias
</commit_message>
<xml_diff>
--- a/Archivos_Excel_Matrices/Matriz de camiones.xlsx
+++ b/Archivos_Excel_Matrices/Matriz de camiones.xlsx
@@ -1,13 +1,8 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="6" rupBuild="4507"/>
   <workbookPr defaultThemeVersion="124226"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Guillermo\Dropbox\Gente\Víctor-Memo\TESIS!!!\Diseño\Nueva distribucion de brete\5. Operaciones\Programación de Rutas\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
   <bookViews>
     <workbookView xWindow="120" yWindow="15" windowWidth="15135" windowHeight="8130"/>
   </bookViews>
@@ -17,7 +12,7 @@
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'Info camiones'!$B$3:$H$21</definedName>
   </definedNames>
-  <calcPr calcId="152511"/>
+  <calcPr calcId="125725"/>
 </workbook>
 </file>
 
@@ -27,7 +22,7 @@
     <author>Guillermo Aguilar</author>
   </authors>
   <commentList>
-    <comment ref="C18" authorId="0" shapeId="0">
+    <comment ref="C18" authorId="0">
       <text>
         <r>
           <rPr>
@@ -56,7 +51,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="17">
   <si>
     <t>Placa</t>
   </si>
@@ -104,13 +99,16 @@
   </si>
   <si>
     <t>Cantidad de camiones</t>
+  </si>
+  <si>
+    <t>Disponibilidad de tiempo(int)</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="6" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <fonts count="6">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -306,7 +304,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
+        <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -338,10 +336,9 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -373,7 +370,6 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -549,17 +545,17 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
   <dimension ref="B2:K21"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="I1" sqref="I1:I1048576"/>
+      <selection activeCell="K17" sqref="K17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="12.75"/>
   <cols>
     <col min="1" max="1" width="3.140625" style="1" customWidth="1"/>
     <col min="2" max="2" width="14.140625" style="1" customWidth="1"/>
@@ -574,7 +570,7 @@
     <col min="11" max="16384" width="11.42578125" style="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:11" x14ac:dyDescent="0.2">
+    <row r="2" spans="2:11">
       <c r="B2" s="11" t="s">
         <v>9</v>
       </c>
@@ -591,7 +587,7 @@
         <v>0.85</v>
       </c>
     </row>
-    <row r="3" spans="2:11" s="7" customFormat="1" ht="27.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="2:11" s="7" customFormat="1" ht="27.75" customHeight="1">
       <c r="B3" s="6" t="s">
         <v>15</v>
       </c>
@@ -613,8 +609,11 @@
       <c r="H3" s="5" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="4" spans="2:11" x14ac:dyDescent="0.2">
+      <c r="I3" s="7" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="4" spans="2:11">
       <c r="B4" s="3">
         <v>1</v>
       </c>
@@ -638,8 +637,11 @@
       <c r="H4" s="8" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="5" spans="2:11" x14ac:dyDescent="0.2">
+      <c r="I4" s="1">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="5" spans="2:11">
       <c r="B5" s="3">
         <v>2</v>
       </c>
@@ -663,8 +665,11 @@
       <c r="H5" s="8" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="6" spans="2:11" x14ac:dyDescent="0.2">
+      <c r="I5" s="1">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="6" spans="2:11">
       <c r="B6" s="3">
         <v>3</v>
       </c>
@@ -688,8 +693,11 @@
       <c r="H6" s="8" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="7" spans="2:11" x14ac:dyDescent="0.2">
+      <c r="I6" s="1">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="7" spans="2:11">
       <c r="B7" s="3">
         <v>4</v>
       </c>
@@ -713,8 +721,11 @@
       <c r="H7" s="8" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="8" spans="2:11" x14ac:dyDescent="0.2">
+      <c r="I7" s="1">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="8" spans="2:11">
       <c r="B8" s="3">
         <v>5</v>
       </c>
@@ -738,8 +749,11 @@
       <c r="H8" s="8" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="9" spans="2:11" x14ac:dyDescent="0.2">
+      <c r="I8" s="1">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="9" spans="2:11">
       <c r="B9" s="3">
         <v>6</v>
       </c>
@@ -763,8 +777,11 @@
       <c r="H9" s="8" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="10" spans="2:11" x14ac:dyDescent="0.2">
+      <c r="I9" s="1">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="10" spans="2:11">
       <c r="B10" s="3">
         <v>7</v>
       </c>
@@ -788,8 +805,11 @@
       <c r="H10" s="8" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="11" spans="2:11" x14ac:dyDescent="0.2">
+      <c r="I10" s="1">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="11" spans="2:11">
       <c r="B11" s="3">
         <v>8</v>
       </c>
@@ -813,8 +833,11 @@
       <c r="H11" s="8" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="12" spans="2:11" x14ac:dyDescent="0.2">
+      <c r="I11" s="1">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="12" spans="2:11">
       <c r="B12" s="3">
         <v>9</v>
       </c>
@@ -838,8 +861,11 @@
       <c r="H12" s="8" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="13" spans="2:11" x14ac:dyDescent="0.2">
+      <c r="I12" s="1">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="13" spans="2:11">
       <c r="B13" s="3">
         <v>10</v>
       </c>
@@ -863,8 +889,11 @@
       <c r="H13" s="8" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="14" spans="2:11" x14ac:dyDescent="0.2">
+      <c r="I13" s="1">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="14" spans="2:11">
       <c r="B14" s="3">
         <v>11</v>
       </c>
@@ -888,8 +917,11 @@
       <c r="H14" s="8" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="15" spans="2:11" x14ac:dyDescent="0.2">
+      <c r="I14" s="1">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="15" spans="2:11">
       <c r="B15" s="3">
         <v>12</v>
       </c>
@@ -913,8 +945,11 @@
       <c r="H15" s="8" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="16" spans="2:11" x14ac:dyDescent="0.2">
+      <c r="I15" s="1">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="16" spans="2:11">
       <c r="B16" s="3">
         <v>13</v>
       </c>
@@ -938,8 +973,11 @@
       <c r="H16" s="8" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="17" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="I16" s="1">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="17" spans="2:9">
       <c r="B17" s="3">
         <v>14</v>
       </c>
@@ -963,8 +1001,11 @@
       <c r="H17" s="8" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="18" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="I17" s="1">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="18" spans="2:9">
       <c r="B18" s="3">
         <v>15</v>
       </c>
@@ -988,8 +1029,11 @@
       <c r="H18" s="8" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="19" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="I18" s="1">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="19" spans="2:9">
       <c r="B19" s="3">
         <v>16</v>
       </c>
@@ -1013,8 +1057,11 @@
       <c r="H19" s="8" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="20" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="I19" s="1">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="20" spans="2:9">
       <c r="B20" s="3">
         <v>17</v>
       </c>
@@ -1035,8 +1082,11 @@
       <c r="H20" s="8" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="21" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="I20" s="1">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="21" spans="2:9">
       <c r="B21" s="3">
         <v>18</v>
       </c>
@@ -1059,6 +1109,9 @@
       </c>
       <c r="H21" s="8" t="s">
         <v>5</v>
+      </c>
+      <c r="I21" s="1">
+        <v>11</v>
       </c>
     </row>
   </sheetData>

</xml_diff>